<commit_message>
improved definitions of hospital markets
</commit_message>
<xml_diff>
--- a/NH_HealthCost_data/29826 Arthroscopic Shoulder Surgery.xlsx
+++ b/NH_HealthCost_data/29826 Arthroscopic Shoulder Surgery.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/teresarokos/Desktop/Thesis Research/Thesis_Hospital_Costs/NH_HealthCost_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D01A0D-F7B8-9345-9EDD-3FEF2E61ABCD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC1C0A6-FFDA-244E-93F4-6FB1BAA7182D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16540" activeTab="4" xr2:uid="{908DF8FC-DA0E-9142-97C3-2981526D7DA1}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16520" activeTab="2" xr2:uid="{908DF8FC-DA0E-9142-97C3-2981526D7DA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Anthem NH" sheetId="1" r:id="rId1"/>
@@ -23621,8 +23621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65B620CF-1798-9D44-BA86-0CFF0C737C5A}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24124,7 +24124,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23E1AB19-B2A1-2D43-8F7A-0C43C5AC3799}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E19"/>
     </sheetView>
   </sheetViews>

</xml_diff>